<commit_message>
Adding new kesy to localization file
</commit_message>
<xml_diff>
--- a/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
+++ b/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Inżynierka\HackSafe\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178BC8FF-C41A-419B-8DC0-8329EE270F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C132A6-9237-467B-9FD1-847710F079CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -81,16 +81,68 @@
   </si>
   <si>
     <t>brutForse</t>
+  </si>
+  <si>
+    <t>cd - change directory</t>
+  </si>
+  <si>
+    <t>ls - list files</t>
+  </si>
+  <si>
+    <t>ssh - connect to device via ssh protocol</t>
+  </si>
+  <si>
+    <t>scp - copy files from remote machines via ssh</t>
+  </si>
+  <si>
+    <t>cd - zmień katalog</t>
+  </si>
+  <si>
+    <t>ls - wyświetl listę plików</t>
+  </si>
+  <si>
+    <t>ssh - połącz się z urządzeniem za pomocą protokołu ssh</t>
+  </si>
+  <si>
+    <t>scp - skopiuj pliki ze zdalnych maszyn za pomocą ssh</t>
+  </si>
+  <si>
+    <t>mkdir - utwórz katalog</t>
+  </si>
+  <si>
+    <t>mkdir - create directory</t>
+  </si>
+  <si>
+    <t>command0</t>
+  </si>
+  <si>
+    <t>command1</t>
+  </si>
+  <si>
+    <t>command2</t>
+  </si>
+  <si>
+    <t>command3</t>
+  </si>
+  <si>
+    <t>command4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -456,11 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3952D7-A9B1-4A2B-A865-60B8FC46C43B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +576,63 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in localization file
</commit_message>
<xml_diff>
--- a/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
+++ b/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Inżynierka\HackSafe\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C132A6-9237-467B-9FD1-847710F079CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F397359-AD66-422C-AE7B-0EDECE19102B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Polish</t>
-  </si>
-  <si>
     <t>&lt;i&gt;bruteForce&lt;/i&gt; - starts brute force programm</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>command4</t>
+  </si>
+  <si>
+    <t>Polski</t>
   </si>
 </sst>
 </file>
@@ -512,16 +512,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,106 +529,106 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing top panel buttons
</commit_message>
<xml_diff>
--- a/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
+++ b/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Inżynierka\HackSafe\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3D9019-51F0-45DD-B270-0FF6BE05A9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC3111-2718-4582-949C-4D7DB8E46AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="136">
   <si>
     <t>Key</t>
   </si>
@@ -408,6 +408,42 @@
   </si>
   <si>
     <t>View of a {0} company network</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>warningLabel_key</t>
+  </si>
+  <si>
+    <t>OSTRZEŻENIE</t>
+  </si>
+  <si>
+    <t>aprove_btn_key</t>
+  </si>
+  <si>
+    <t>disaporve_btn_key</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Tak</t>
+  </si>
+  <si>
+    <t>Nie</t>
+  </si>
+  <si>
+    <t>exitSystemMEssage_key</t>
+  </si>
+  <si>
+    <t>Are you sure you want to exit HackSafe system?</t>
+  </si>
+  <si>
+    <t>Czy na pewno chcesz opuścić HackSafe system?</t>
   </si>
 </sst>
 </file>
@@ -790,11 +826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3952D7-A9B1-4A2B-A865-60B8FC46C43B}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,111 +1194,155 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding pop up message overlay and adding linux comments descriptions inti glosary
</commit_message>
<xml_diff>
--- a/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
+++ b/HackSafe/Assets/Resources/LocalizationExcelSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Inżynierka\HackSafe\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AC3111-2718-4582-949C-4D7DB8E46AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2027EB55-7C8C-4CD0-9EC0-C87F38E7AEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C244F3DC-1BA1-4A4A-B6A1-7B35F6450258}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
   <si>
     <t>Key</t>
   </si>
@@ -444,13 +444,235 @@
   </si>
   <si>
     <t>Czy na pewno chcesz opuścić HackSafe system?</t>
+  </si>
+  <si>
+    <t>cd comment</t>
+  </si>
+  <si>
+    <t>cdCommand_title</t>
+  </si>
+  <si>
+    <t>Polecenie cd</t>
+  </si>
+  <si>
+    <t>ls commend</t>
+  </si>
+  <si>
+    <t>Polecenie ls</t>
+  </si>
+  <si>
+    <t>The ls command writes to standard output the contents of each specified Directory parameter or the name of each specified File parameter. If you do not specify a File or Directory parameter, the ls command displays the contents of the current directory.</t>
+  </si>
+  <si>
+    <t>Polecenie ls wyświetla na standardowym wyjściu zawartość każdego określonego w parametrach katalogu lub nazwę każdego określonego parametrem pliku. Jeżeli nie określono w parametrach pliku lub katalogu, polecenie ls wyświetla zawartość bieżącego katalogu.</t>
+  </si>
+  <si>
+    <t>lsCommand_title</t>
+  </si>
+  <si>
+    <t>lsCommand_content</t>
+  </si>
+  <si>
+    <t>cat commend</t>
+  </si>
+  <si>
+    <t>Polecenie cat</t>
+  </si>
+  <si>
+    <t>ssh commend</t>
+  </si>
+  <si>
+    <t>Polecenie ssh</t>
+  </si>
+  <si>
+    <t>scp command</t>
+  </si>
+  <si>
+    <t>Polecenie scp</t>
+  </si>
+  <si>
+    <t>scpCommand_title</t>
+  </si>
+  <si>
+    <t>sshCommand_title</t>
+  </si>
+  <si>
+    <t>catCommand_title</t>
+  </si>
+  <si>
+    <t>mkdirCommand_title</t>
+  </si>
+  <si>
+    <t>mkdir command</t>
+  </si>
+  <si>
+    <t>Polecenie mkdir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cd: The cd command will allow you to change directories. When you open a terminal you will be in your home directory. To move around the file system you will use cd. Examples: </t>
+  </si>
+  <si>
+    <t>cdCommand_content_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To navigate into the root directory, use $ cd / </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To navigate to your home directory, use $ cd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To navigate up one directory level, use $ cd .. </t>
+  </si>
+  <si>
+    <t>To navigate through multiple levels of directory at once, specify the full directory path that you want to go to. For example, use, $ cd /var/www to go directly to the /www subdirectory of /var/.</t>
+  </si>
+  <si>
+    <t>cdCommand_content_2</t>
+  </si>
+  <si>
+    <t>cdCommand_content_3</t>
+  </si>
+  <si>
+    <t>cdCommand_content_4</t>
+  </si>
+  <si>
+    <t>cdCommand_content_5</t>
+  </si>
+  <si>
+    <t>cd: Polecenie cd umożliwia zmianę katalogów. Po otwarciu terminala znajdziesz się w swoim katalogu domowym. Aby poruszać się po systemie plików, użyj polecenia cd. Przykłady:</t>
+  </si>
+  <si>
+    <t>Aby przejść do katalogu głównego, użyj polecenia $ cd /</t>
+  </si>
+  <si>
+    <t>Aby przejść do katalogu domowego, użyj polecenia $ cd</t>
+  </si>
+  <si>
+    <t>Aby przejść o jeden poziom wyżej w katalogu, użyj polecenia $cd</t>
+  </si>
+  <si>
+    <t>Aby przejść przez wiele poziomów katalogu jednocześnie, określ pełną ścieżkę do katalogu, do którego chcesz przejść. Na przykład użyj polecenia  $ cd /var/www, aby przejść bezpośrednio do podkatalogu /www w katalogu /var/.</t>
+  </si>
+  <si>
+    <t>This command displays the data in the notes file.</t>
+  </si>
+  <si>
+    <t>The cat command reads each File parameter in sequence and writes it to standard output. To display a file at the workstation, enter:</t>
+  </si>
+  <si>
+    <t>$ cat notes</t>
+  </si>
+  <si>
+    <t>To polecenie wyświetla dane w pliku notes.</t>
+  </si>
+  <si>
+    <t>Polecenie cat odczytuje każdy parametr pliku w sekwencji i wypisuje go na standardowym wyjściu. Aby wyświetlić plik na stacji roboczej, wprowadź:</t>
+  </si>
+  <si>
+    <t>ssh (SSH client) is a program for logging into a remote machine and for executing commands on a remote machine. It is intended to provide secure encrypted communications between two untrusted hosts over an insecure network. X11 connections, arbitrary TCP ports and UNIX-domain sockets can also be forwarded over the secure channel.</t>
+  </si>
+  <si>
+    <t>ssh connects and logs into the specified destination, which is specified as user@host_ip. The user must prove their identity to the remote machine using password.</t>
+  </si>
+  <si>
+    <t>ssh (SSH client) to program do logowania się do zdalnej maszyny i wykonywania poleceń na zdalnej maszynie. Jego celem jest zapewnienie bezpiecznej szyfrowanej komunikacji między dwoma niezaufanymi hostami przez niezabezpieczoną sieć. Połączenia X11, dowolne porty TCP i gniazda domeny UNIX mogą być również przekazywane przez bezpieczny kanał.</t>
+  </si>
+  <si>
+    <t>ssh łączy się i loguje do określonego miejsca docelowego, które jest określone jako user@host_ip. Użytkownik musi udowodnić swoją tożsamość zdalnej maszynie za pomocą hasła.</t>
+  </si>
+  <si>
+    <t>scp copies files between hosts on a network. It uses ssh for data transfer, and uses the same authentication and provides the same security as ssh. scp will ask for passwords or passphrases if they are needed for authentication.</t>
+  </si>
+  <si>
+    <t>Examples:</t>
+  </si>
+  <si>
+    <t>$ scp your_username@remotehost.edu:foobar.txt /some/local/directory</t>
+  </si>
+  <si>
+    <t>Copy the file \"foobar.txt\" from the local host to a remote host:</t>
+  </si>
+  <si>
+    <t>$ scp foobar.txt your_username@remotehost.edu:/some/remote/directory</t>
+  </si>
+  <si>
+    <t>scpCommand_content_1</t>
+  </si>
+  <si>
+    <t>scpCommand_content_2</t>
+  </si>
+  <si>
+    <t>scpCommand_content_3</t>
+  </si>
+  <si>
+    <t>scpCommand_content_4</t>
+  </si>
+  <si>
+    <t>scpCommand_content_5</t>
+  </si>
+  <si>
+    <t>scpCommand_content_6</t>
+  </si>
+  <si>
+    <t>scp kopiuje pliki między hostami w sieci. Używa ssh do przesyłania danych i używa tego samego uwierzytelniania i zapewnia takie samo bezpieczeństwo jak ssh. scp poprosi o hasła lub frazy-hasła, jeśli są potrzebne do uwierzytelnienia.</t>
+  </si>
+  <si>
+    <t>Przykłady:</t>
+  </si>
+  <si>
+    <t>Skopiuj plik foobar.txt z lokalnego hosta na zdalny host:</t>
+  </si>
+  <si>
+    <t>Skopiuj plik foobar.txt ze zdalnego hosta na lokalny:</t>
+  </si>
+  <si>
+    <t>Copy the file foobar.txt from a remote host to the local host:</t>
+  </si>
+  <si>
+    <t>The mkdir command creates one or more new directories specified by the Directory parameter.</t>
+  </si>
+  <si>
+    <t>To create a new directory called Test in the current working directory, enter:</t>
+  </si>
+  <si>
+    <t>$ mkdir Test</t>
+  </si>
+  <si>
+    <t>Polecenie mkdir tworzy jeden lub więcej nowych katalogów określonych przez parametr Directory.</t>
+  </si>
+  <si>
+    <t>Aby utworzyć nowy katalog o nazwie Test w bieżącym katalogu roboczym, należy wywołać polecenie:</t>
+  </si>
+  <si>
+    <t>mkdirCommand_content_1</t>
+  </si>
+  <si>
+    <t>mkdirCommand_content_2</t>
+  </si>
+  <si>
+    <t>mkdirCommand_content_3</t>
+  </si>
+  <si>
+    <t>sshCommand_content_1</t>
+  </si>
+  <si>
+    <t>sshCommand_content_2</t>
+  </si>
+  <si>
+    <t>catCommand_content_1</t>
+  </si>
+  <si>
+    <t>catCommand_content_2</t>
+  </si>
+  <si>
+    <t>catCommand_content_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +683,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -484,16 +715,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -826,11 +1063,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3952D7-A9B1-4A2B-A865-60B8FC46C43B}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1429,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>125</v>
       </c>
@@ -1203,7 +1440,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -1214,7 +1451,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -1225,7 +1462,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>133</v>
       </c>
@@ -1236,118 +1473,437 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>166</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>208</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>209</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>203</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>